<commit_message>
added SOM saving as png file
</commit_message>
<xml_diff>
--- a/SOMNeuronDistances.xlsx
+++ b/SOMNeuronDistances.xlsx
@@ -388,16 +388,16 @@
         <v>0.15</v>
       </c>
       <c r="B2">
-        <v>4446.61</v>
+        <v>4392.86</v>
       </c>
       <c r="C2">
-        <v>134.75</v>
+        <v>133.12</v>
       </c>
       <c r="D2">
-        <v>4915.97</v>
+        <v>4901.9</v>
       </c>
       <c r="E2">
-        <v>148.97</v>
+        <v>148.54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -405,16 +405,16 @@
         <v>0.15</v>
       </c>
       <c r="B3">
-        <v>4672.72</v>
+        <v>4837.83</v>
       </c>
       <c r="C3">
-        <v>141.6</v>
+        <v>146.6</v>
       </c>
       <c r="D3">
-        <v>607.29</v>
+        <v>606.73</v>
       </c>
       <c r="E3">
-        <v>18.4</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -422,16 +422,16 @@
         <v>0.15</v>
       </c>
       <c r="B4">
-        <v>226.11</v>
+        <v>444.97</v>
       </c>
       <c r="C4">
-        <v>6.85</v>
+        <v>13.48</v>
       </c>
       <c r="D4">
-        <v>-4308.68</v>
+        <v>-4295.17</v>
       </c>
       <c r="E4">
-        <v>-130.57</v>
+        <v>-130.15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -439,16 +439,16 @@
         <v>0.1</v>
       </c>
       <c r="B5">
-        <v>4432.39</v>
+        <v>4435.8</v>
       </c>
       <c r="C5">
-        <v>134.31</v>
+        <v>134.42</v>
       </c>
       <c r="D5">
-        <v>5011.41</v>
+        <v>5120.98</v>
       </c>
       <c r="E5">
-        <v>151.86</v>
+        <v>155.18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -456,16 +456,16 @@
         <v>0.1</v>
       </c>
       <c r="B6">
-        <v>996.6</v>
+        <v>899.52</v>
       </c>
       <c r="C6">
-        <v>30.2</v>
+        <v>27.26</v>
       </c>
       <c r="D6">
-        <v>1070.57</v>
+        <v>1131.7</v>
       </c>
       <c r="E6">
-        <v>32.44</v>
+        <v>34.29</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -473,16 +473,16 @@
         <v>0.1</v>
       </c>
       <c r="B7">
-        <v>-3435.79</v>
+        <v>-3536.28</v>
       </c>
       <c r="C7">
-        <v>-104.11</v>
+        <v>-107.16</v>
       </c>
       <c r="D7">
-        <v>-3940.84</v>
+        <v>-3989.28</v>
       </c>
       <c r="E7">
-        <v>-119.42</v>
+        <v>-120.89</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -490,16 +490,16 @@
         <v>0.01</v>
       </c>
       <c r="B8">
-        <v>4877.99</v>
+        <v>4817.45</v>
       </c>
       <c r="C8">
-        <v>147.82</v>
+        <v>145.98</v>
       </c>
       <c r="D8">
-        <v>4719.88</v>
+        <v>4808.9</v>
       </c>
       <c r="E8">
-        <v>143.03</v>
+        <v>145.72</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -507,16 +507,16 @@
         <v>0.01</v>
       </c>
       <c r="B9">
-        <v>2963.81</v>
+        <v>2928.13</v>
       </c>
       <c r="C9">
-        <v>89.81</v>
+        <v>88.73</v>
       </c>
       <c r="D9">
-        <v>2841.43</v>
+        <v>2889.89</v>
       </c>
       <c r="E9">
-        <v>86.09999999999999</v>
+        <v>87.56999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -524,16 +524,16 @@
         <v>0.01</v>
       </c>
       <c r="B10">
-        <v>-1914.18</v>
+        <v>-1889.32</v>
       </c>
       <c r="C10">
-        <v>-58.01</v>
+        <v>-57.25</v>
       </c>
       <c r="D10">
-        <v>-1878.45</v>
+        <v>-1919.01</v>
       </c>
       <c r="E10">
-        <v>-56.93</v>
+        <v>-58.15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -541,16 +541,16 @@
         <v>0.001</v>
       </c>
       <c r="B11">
-        <v>1296.88</v>
+        <v>1373</v>
       </c>
       <c r="C11">
-        <v>39.3</v>
+        <v>41.61</v>
       </c>
       <c r="D11">
-        <v>2714.55</v>
+        <v>2614.63</v>
       </c>
       <c r="E11">
-        <v>82.26000000000001</v>
+        <v>79.23</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -558,16 +558,16 @@
         <v>0.001</v>
       </c>
       <c r="B12">
-        <v>2728.76</v>
+        <v>2753.59</v>
       </c>
       <c r="C12">
-        <v>82.69</v>
+        <v>83.44</v>
       </c>
       <c r="D12">
-        <v>1830.71</v>
+        <v>1801.63</v>
       </c>
       <c r="E12">
-        <v>55.48</v>
+        <v>54.59</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -575,16 +575,16 @@
         <v>0.001</v>
       </c>
       <c r="B13">
-        <v>1431.88</v>
+        <v>1380.59</v>
       </c>
       <c r="C13">
-        <v>43.39</v>
+        <v>41.83</v>
       </c>
       <c r="D13">
-        <v>-883.84</v>
+        <v>-813</v>
       </c>
       <c r="E13">
-        <v>-26.78</v>
+        <v>-24.64</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -592,16 +592,16 @@
         <v>0.0001</v>
       </c>
       <c r="B14">
-        <v>831.13</v>
+        <v>808.87</v>
       </c>
       <c r="C14">
-        <v>25.19</v>
+        <v>24.51</v>
       </c>
       <c r="D14">
-        <v>877.5700000000001</v>
+        <v>935.24</v>
       </c>
       <c r="E14">
-        <v>26.59</v>
+        <v>28.34</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -609,16 +609,16 @@
         <v>0.0001</v>
       </c>
       <c r="B15">
-        <v>878.73</v>
+        <v>817.63</v>
       </c>
       <c r="C15">
-        <v>26.63</v>
+        <v>24.78</v>
       </c>
       <c r="D15">
-        <v>813.41</v>
+        <v>810.4</v>
       </c>
       <c r="E15">
-        <v>24.65</v>
+        <v>24.56</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -626,16 +626,16 @@
         <v>0.0001</v>
       </c>
       <c r="B16">
-        <v>47.6</v>
+        <v>8.76</v>
       </c>
       <c r="C16">
-        <v>1.44</v>
+        <v>0.27</v>
       </c>
       <c r="D16">
-        <v>-64.16</v>
+        <v>-124.84</v>
       </c>
       <c r="E16">
-        <v>-1.94</v>
+        <v>-3.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added writing data types at the beggingi of each row in xlsx file
</commit_message>
<xml_diff>
--- a/SOMNeuronDistances.xlsx
+++ b/SOMNeuronDistances.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+  <si>
+    <t>DataType</t>
+  </si>
   <si>
     <t>LearningRate</t>
   </si>
@@ -29,6 +32,15 @@
   </si>
   <si>
     <t>avgAgainst</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -360,13 +372,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,260 +394,263 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>0.15</v>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>4392.86</v>
+        <v>4330.81</v>
       </c>
       <c r="C2">
-        <v>133.12</v>
+        <v>131.24</v>
       </c>
       <c r="D2">
-        <v>4901.9</v>
+        <v>4915.63</v>
       </c>
       <c r="E2">
-        <v>148.54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0.15</v>
+        <v>148.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>4837.83</v>
+        <v>4837.29</v>
       </c>
       <c r="C3">
-        <v>146.6</v>
+        <v>146.58</v>
       </c>
       <c r="D3">
-        <v>606.73</v>
+        <v>505.07</v>
       </c>
       <c r="E3">
-        <v>18.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>0.15</v>
+        <v>15.31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>444.97</v>
+        <v>506.48</v>
       </c>
       <c r="C4">
-        <v>13.48</v>
+        <v>15.34</v>
       </c>
       <c r="D4">
-        <v>-4295.17</v>
+        <v>-4410.56</v>
       </c>
       <c r="E4">
-        <v>-130.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>0.1</v>
+        <v>-133.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>4435.8</v>
+        <v>4389.36</v>
       </c>
       <c r="C5">
-        <v>134.42</v>
+        <v>133.01</v>
       </c>
       <c r="D5">
-        <v>5120.98</v>
+        <v>5074.63</v>
       </c>
       <c r="E5">
-        <v>155.18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>0.1</v>
+        <v>153.78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>899.52</v>
+        <v>846.51</v>
       </c>
       <c r="C6">
-        <v>27.26</v>
+        <v>25.65</v>
       </c>
       <c r="D6">
-        <v>1131.7</v>
+        <v>1050.26</v>
       </c>
       <c r="E6">
-        <v>34.29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>0.1</v>
+        <v>31.83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>-3536.28</v>
+        <v>-3542.85</v>
       </c>
       <c r="C7">
-        <v>-107.16</v>
+        <v>-107.36</v>
       </c>
       <c r="D7">
-        <v>-3989.28</v>
+        <v>-4024.37</v>
       </c>
       <c r="E7">
-        <v>-120.89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>0.01</v>
+        <v>-121.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>4817.45</v>
+        <v>5003.86</v>
       </c>
       <c r="C8">
-        <v>145.98</v>
+        <v>151.63</v>
       </c>
       <c r="D8">
-        <v>4808.9</v>
+        <v>4612.07</v>
       </c>
       <c r="E8">
-        <v>145.72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>0.01</v>
+        <v>139.76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>2928.13</v>
+        <v>2904.51</v>
       </c>
       <c r="C9">
-        <v>88.73</v>
+        <v>88.02</v>
       </c>
       <c r="D9">
-        <v>2889.89</v>
+        <v>2895.74</v>
       </c>
       <c r="E9">
-        <v>87.56999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>0.01</v>
+        <v>87.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>-1889.32</v>
+        <v>-2099.35</v>
       </c>
       <c r="C10">
-        <v>-57.25</v>
+        <v>-63.61</v>
       </c>
       <c r="D10">
-        <v>-1919.01</v>
+        <v>-1716.33</v>
       </c>
       <c r="E10">
-        <v>-58.15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>0.001</v>
+        <v>-52.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>1373</v>
+        <v>1389.59</v>
       </c>
       <c r="C11">
-        <v>41.61</v>
+        <v>42.11</v>
       </c>
       <c r="D11">
-        <v>2614.63</v>
+        <v>2778.19</v>
       </c>
       <c r="E11">
-        <v>79.23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>0.001</v>
+        <v>84.19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>2753.59</v>
+        <v>2662.86</v>
       </c>
       <c r="C12">
-        <v>83.44</v>
+        <v>80.69</v>
       </c>
       <c r="D12">
-        <v>1801.63</v>
+        <v>1736.37</v>
       </c>
       <c r="E12">
-        <v>54.59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>0.001</v>
+        <v>52.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>1380.59</v>
+        <v>1273.27</v>
       </c>
       <c r="C13">
-        <v>41.83</v>
+        <v>38.58</v>
       </c>
       <c r="D13">
-        <v>-813</v>
+        <v>-1041.82</v>
       </c>
       <c r="E13">
-        <v>-24.64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>0.0001</v>
+        <v>-31.57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>808.87</v>
+        <v>759.74</v>
       </c>
       <c r="C14">
-        <v>24.51</v>
+        <v>23.02</v>
       </c>
       <c r="D14">
-        <v>935.24</v>
+        <v>839.87</v>
       </c>
       <c r="E14">
-        <v>28.34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>0.0001</v>
+        <v>25.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>817.63</v>
+        <v>869.1900000000001</v>
       </c>
       <c r="C15">
-        <v>24.78</v>
+        <v>26.34</v>
       </c>
       <c r="D15">
-        <v>810.4</v>
+        <v>736.4</v>
       </c>
       <c r="E15">
-        <v>24.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>0.0001</v>
+        <v>22.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>8.76</v>
+        <v>109.45</v>
       </c>
       <c r="C16">
-        <v>0.27</v>
+        <v>3.32</v>
       </c>
       <c r="D16">
-        <v>-124.84</v>
+        <v>-103.47</v>
       </c>
       <c r="E16">
-        <v>-3.78</v>
+        <v>-3.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed data writiing issues
</commit_message>
<xml_diff>
--- a/SOMNeuronDistances.xlsx
+++ b/SOMNeuronDistances.xlsx
@@ -403,16 +403,16 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>4330.81</v>
+        <v>0.15</v>
       </c>
       <c r="C2">
-        <v>131.24</v>
+        <v>4350.22</v>
       </c>
       <c r="D2">
-        <v>4915.63</v>
+        <v>131.82</v>
       </c>
       <c r="E2">
-        <v>148.96</v>
+        <v>4797.24</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -420,16 +420,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>4837.29</v>
+        <v>0.15</v>
       </c>
       <c r="C3">
-        <v>146.58</v>
+        <v>4749.3</v>
       </c>
       <c r="D3">
-        <v>505.07</v>
+        <v>143.92</v>
       </c>
       <c r="E3">
-        <v>15.31</v>
+        <v>542.73</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -437,16 +437,16 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>506.48</v>
+        <v>0.15</v>
       </c>
       <c r="C4">
-        <v>15.34</v>
+        <v>399.08</v>
       </c>
       <c r="D4">
-        <v>-4410.56</v>
+        <v>12.1</v>
       </c>
       <c r="E4">
-        <v>-133.65</v>
+        <v>-4254.51</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -454,16 +454,16 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>4389.36</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>133.01</v>
+        <v>4513.4</v>
       </c>
       <c r="D5">
-        <v>5074.63</v>
+        <v>136.77</v>
       </c>
       <c r="E5">
-        <v>153.78</v>
+        <v>4990.83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -471,16 +471,16 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>846.51</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>25.65</v>
+        <v>985.39</v>
       </c>
       <c r="D6">
-        <v>1050.26</v>
+        <v>29.86</v>
       </c>
       <c r="E6">
-        <v>31.83</v>
+        <v>1018.67</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -488,16 +488,16 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>-3542.85</v>
+        <v>0.1</v>
       </c>
       <c r="C7">
-        <v>-107.36</v>
+        <v>-3528.01</v>
       </c>
       <c r="D7">
-        <v>-4024.37</v>
+        <v>-106.91</v>
       </c>
       <c r="E7">
-        <v>-121.95</v>
+        <v>-3972.16</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -505,16 +505,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5003.86</v>
+        <v>0.01</v>
       </c>
       <c r="C8">
-        <v>151.63</v>
+        <v>4764.56</v>
       </c>
       <c r="D8">
-        <v>4612.07</v>
+        <v>144.38</v>
       </c>
       <c r="E8">
-        <v>139.76</v>
+        <v>4692.04</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -522,16 +522,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2904.51</v>
+        <v>0.01</v>
       </c>
       <c r="C9">
-        <v>88.02</v>
+        <v>2736.93</v>
       </c>
       <c r="D9">
-        <v>2895.74</v>
+        <v>82.94</v>
       </c>
       <c r="E9">
-        <v>87.75</v>
+        <v>2967.03</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -539,16 +539,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-2099.35</v>
+        <v>0.01</v>
       </c>
       <c r="C10">
-        <v>-63.61</v>
+        <v>-2027.63</v>
       </c>
       <c r="D10">
-        <v>-1716.33</v>
+        <v>-61.44</v>
       </c>
       <c r="E10">
-        <v>-52.01</v>
+        <v>-1725.01</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -556,16 +556,16 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>1389.59</v>
+        <v>0.001</v>
       </c>
       <c r="C11">
-        <v>42.11</v>
+        <v>1300.78</v>
       </c>
       <c r="D11">
-        <v>2778.19</v>
+        <v>39.42</v>
       </c>
       <c r="E11">
-        <v>84.19</v>
+        <v>2735.17</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -573,16 +573,16 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>2662.86</v>
+        <v>0.001</v>
       </c>
       <c r="C12">
-        <v>80.69</v>
+        <v>2662.31</v>
       </c>
       <c r="D12">
-        <v>1736.37</v>
+        <v>80.68000000000001</v>
       </c>
       <c r="E12">
-        <v>52.62</v>
+        <v>1689.51</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -590,16 +590,16 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>1273.27</v>
+        <v>0.001</v>
       </c>
       <c r="C13">
-        <v>38.58</v>
+        <v>1361.53</v>
       </c>
       <c r="D13">
-        <v>-1041.82</v>
+        <v>41.26</v>
       </c>
       <c r="E13">
-        <v>-31.57</v>
+        <v>-1045.66</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -607,16 +607,16 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>759.74</v>
+        <v>0.0001</v>
       </c>
       <c r="C14">
-        <v>23.02</v>
+        <v>724.1900000000001</v>
       </c>
       <c r="D14">
-        <v>839.87</v>
+        <v>21.95</v>
       </c>
       <c r="E14">
-        <v>25.45</v>
+        <v>920.91</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -624,16 +624,16 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>869.1900000000001</v>
+        <v>0.0001</v>
       </c>
       <c r="C15">
-        <v>26.34</v>
+        <v>864.77</v>
       </c>
       <c r="D15">
-        <v>736.4</v>
+        <v>26.21</v>
       </c>
       <c r="E15">
-        <v>22.32</v>
+        <v>784.4400000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -641,16 +641,16 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <v>109.45</v>
+        <v>0.0001</v>
       </c>
       <c r="C16">
-        <v>3.32</v>
+        <v>140.58</v>
       </c>
       <c r="D16">
-        <v>-103.47</v>
+        <v>4.26</v>
       </c>
       <c r="E16">
-        <v>-3.13</v>
+        <v>-136.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally fixed sata writing issues :)
</commit_message>
<xml_diff>
--- a/SOMNeuronDistances.xlsx
+++ b/SOMNeuronDistances.xlsx
@@ -406,13 +406,16 @@
         <v>0.15</v>
       </c>
       <c r="C2">
-        <v>4350.22</v>
+        <v>4254.42</v>
       </c>
       <c r="D2">
-        <v>131.82</v>
+        <v>128.92</v>
       </c>
       <c r="E2">
-        <v>4797.24</v>
+        <v>4898.61</v>
+      </c>
+      <c r="F2">
+        <v>148.44</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -423,13 +426,16 @@
         <v>0.15</v>
       </c>
       <c r="C3">
-        <v>4749.3</v>
+        <v>4704.82</v>
       </c>
       <c r="D3">
-        <v>143.92</v>
+        <v>142.57</v>
       </c>
       <c r="E3">
-        <v>542.73</v>
+        <v>531.65</v>
+      </c>
+      <c r="F3">
+        <v>16.11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -440,13 +446,16 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>399.08</v>
+        <v>450.4</v>
       </c>
       <c r="D4">
-        <v>12.1</v>
+        <v>13.65</v>
       </c>
       <c r="E4">
-        <v>-4254.51</v>
+        <v>-4366.96</v>
+      </c>
+      <c r="F4">
+        <v>-132.33</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -457,13 +466,16 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>4513.4</v>
+        <v>4493.85</v>
       </c>
       <c r="D5">
-        <v>136.77</v>
+        <v>136.18</v>
       </c>
       <c r="E5">
-        <v>4990.83</v>
+        <v>4996.53</v>
+      </c>
+      <c r="F5">
+        <v>151.41</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -474,13 +486,16 @@
         <v>0.1</v>
       </c>
       <c r="C6">
-        <v>985.39</v>
+        <v>921.47</v>
       </c>
       <c r="D6">
-        <v>29.86</v>
+        <v>27.92</v>
       </c>
       <c r="E6">
-        <v>1018.67</v>
+        <v>1171.22</v>
+      </c>
+      <c r="F6">
+        <v>35.49</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -491,13 +506,16 @@
         <v>0.1</v>
       </c>
       <c r="C7">
-        <v>-3528.01</v>
+        <v>-3572.38</v>
       </c>
       <c r="D7">
-        <v>-106.91</v>
+        <v>-108.26</v>
       </c>
       <c r="E7">
-        <v>-3972.16</v>
+        <v>-3825.31</v>
+      </c>
+      <c r="F7">
+        <v>-115.92</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -508,13 +526,16 @@
         <v>0.01</v>
       </c>
       <c r="C8">
-        <v>4764.56</v>
+        <v>5065.24</v>
       </c>
       <c r="D8">
-        <v>144.38</v>
+        <v>153.49</v>
       </c>
       <c r="E8">
-        <v>4692.04</v>
+        <v>4682.85</v>
+      </c>
+      <c r="F8">
+        <v>141.9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -525,13 +546,16 @@
         <v>0.01</v>
       </c>
       <c r="C9">
-        <v>2736.93</v>
+        <v>2787.75</v>
       </c>
       <c r="D9">
-        <v>82.94</v>
+        <v>84.48</v>
       </c>
       <c r="E9">
-        <v>2967.03</v>
+        <v>2899.46</v>
+      </c>
+      <c r="F9">
+        <v>87.86</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -542,13 +566,16 @@
         <v>0.01</v>
       </c>
       <c r="C10">
-        <v>-2027.63</v>
+        <v>-2277.49</v>
       </c>
       <c r="D10">
-        <v>-61.44</v>
+        <v>-69.01000000000001</v>
       </c>
       <c r="E10">
-        <v>-1725.01</v>
+        <v>-1783.39</v>
+      </c>
+      <c r="F10">
+        <v>-54.04</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -559,13 +586,16 @@
         <v>0.001</v>
       </c>
       <c r="C11">
-        <v>1300.78</v>
+        <v>1373.73</v>
       </c>
       <c r="D11">
-        <v>39.42</v>
+        <v>41.63</v>
       </c>
       <c r="E11">
-        <v>2735.17</v>
+        <v>2634.37</v>
+      </c>
+      <c r="F11">
+        <v>79.83</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -576,13 +606,16 @@
         <v>0.001</v>
       </c>
       <c r="C12">
-        <v>2662.31</v>
+        <v>2674.61</v>
       </c>
       <c r="D12">
-        <v>80.68000000000001</v>
+        <v>81.05</v>
       </c>
       <c r="E12">
-        <v>1689.51</v>
+        <v>1766.54</v>
+      </c>
+      <c r="F12">
+        <v>53.53</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -593,13 +626,16 @@
         <v>0.001</v>
       </c>
       <c r="C13">
-        <v>1361.53</v>
+        <v>1300.88</v>
       </c>
       <c r="D13">
-        <v>41.26</v>
+        <v>39.42</v>
       </c>
       <c r="E13">
-        <v>-1045.66</v>
+        <v>-867.83</v>
+      </c>
+      <c r="F13">
+        <v>-26.3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -610,13 +646,16 @@
         <v>0.0001</v>
       </c>
       <c r="C14">
-        <v>724.1900000000001</v>
+        <v>808.88</v>
       </c>
       <c r="D14">
-        <v>21.95</v>
+        <v>24.51</v>
       </c>
       <c r="E14">
-        <v>920.91</v>
+        <v>887.59</v>
+      </c>
+      <c r="F14">
+        <v>26.9</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -627,13 +666,16 @@
         <v>0.0001</v>
       </c>
       <c r="C15">
-        <v>864.77</v>
+        <v>930.39</v>
       </c>
       <c r="D15">
-        <v>26.21</v>
+        <v>28.19</v>
       </c>
       <c r="E15">
-        <v>784.4400000000001</v>
+        <v>740.04</v>
+      </c>
+      <c r="F15">
+        <v>22.43</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -644,13 +686,16 @@
         <v>0.0001</v>
       </c>
       <c r="C16">
-        <v>140.58</v>
+        <v>121.51</v>
       </c>
       <c r="D16">
-        <v>4.26</v>
+        <v>3.68</v>
       </c>
       <c r="E16">
-        <v>-136.47</v>
+        <v>-147.55</v>
+      </c>
+      <c r="F16">
+        <v>-4.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update gitignore for xlsx files
</commit_message>
<xml_diff>
--- a/SOMNeuronDistances.xlsx
+++ b/SOMNeuronDistances.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="newSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -406,16 +406,16 @@
         <v>0.15</v>
       </c>
       <c r="C2">
-        <v>4254.42</v>
+        <v>4399.13</v>
       </c>
       <c r="D2">
-        <v>128.92</v>
+        <v>133.31</v>
       </c>
       <c r="E2">
-        <v>4898.61</v>
+        <v>4998.47</v>
       </c>
       <c r="F2">
-        <v>148.44</v>
+        <v>151.47</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -426,16 +426,16 @@
         <v>0.15</v>
       </c>
       <c r="C3">
-        <v>4704.82</v>
+        <v>4792.82</v>
       </c>
       <c r="D3">
-        <v>142.57</v>
+        <v>145.24</v>
       </c>
       <c r="E3">
-        <v>531.65</v>
+        <v>564.22</v>
       </c>
       <c r="F3">
-        <v>16.11</v>
+        <v>17.1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -446,16 +446,16 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>450.4</v>
+        <v>393.69</v>
       </c>
       <c r="D4">
-        <v>13.65</v>
+        <v>11.93</v>
       </c>
       <c r="E4">
-        <v>-4366.96</v>
+        <v>-4434.25</v>
       </c>
       <c r="F4">
-        <v>-132.33</v>
+        <v>-134.37</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -466,16 +466,16 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>4493.85</v>
+        <v>4485.64</v>
       </c>
       <c r="D5">
-        <v>136.18</v>
+        <v>135.93</v>
       </c>
       <c r="E5">
-        <v>4996.53</v>
+        <v>5084.7</v>
       </c>
       <c r="F5">
-        <v>151.41</v>
+        <v>154.08</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -486,16 +486,16 @@
         <v>0.1</v>
       </c>
       <c r="C6">
-        <v>921.47</v>
+        <v>982.0700000000001</v>
       </c>
       <c r="D6">
-        <v>27.92</v>
+        <v>29.76</v>
       </c>
       <c r="E6">
-        <v>1171.22</v>
+        <v>1147.3</v>
       </c>
       <c r="F6">
-        <v>35.49</v>
+        <v>34.77</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -506,16 +506,16 @@
         <v>0.1</v>
       </c>
       <c r="C7">
-        <v>-3572.38</v>
+        <v>-3503.57</v>
       </c>
       <c r="D7">
-        <v>-108.26</v>
+        <v>-106.17</v>
       </c>
       <c r="E7">
-        <v>-3825.31</v>
+        <v>-3937.4</v>
       </c>
       <c r="F7">
-        <v>-115.92</v>
+        <v>-119.31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -526,16 +526,16 @@
         <v>0.01</v>
       </c>
       <c r="C8">
-        <v>5065.24</v>
+        <v>4871.58</v>
       </c>
       <c r="D8">
-        <v>153.49</v>
+        <v>147.62</v>
       </c>
       <c r="E8">
-        <v>4682.85</v>
+        <v>4649.2</v>
       </c>
       <c r="F8">
-        <v>141.9</v>
+        <v>140.88</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -546,16 +546,16 @@
         <v>0.01</v>
       </c>
       <c r="C9">
-        <v>2787.75</v>
+        <v>2880.57</v>
       </c>
       <c r="D9">
-        <v>84.48</v>
+        <v>87.29000000000001</v>
       </c>
       <c r="E9">
-        <v>2899.46</v>
+        <v>2859.85</v>
       </c>
       <c r="F9">
-        <v>87.86</v>
+        <v>86.66</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -566,16 +566,16 @@
         <v>0.01</v>
       </c>
       <c r="C10">
-        <v>-2277.49</v>
+        <v>-1991.01</v>
       </c>
       <c r="D10">
-        <v>-69.01000000000001</v>
+        <v>-60.33</v>
       </c>
       <c r="E10">
-        <v>-1783.39</v>
+        <v>-1789.35</v>
       </c>
       <c r="F10">
-        <v>-54.04</v>
+        <v>-54.22</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -586,16 +586,16 @@
         <v>0.001</v>
       </c>
       <c r="C11">
-        <v>1373.73</v>
+        <v>1266.52</v>
       </c>
       <c r="D11">
-        <v>41.63</v>
+        <v>38.38</v>
       </c>
       <c r="E11">
-        <v>2634.37</v>
+        <v>2759.79</v>
       </c>
       <c r="F11">
-        <v>79.83</v>
+        <v>83.63</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -606,16 +606,16 @@
         <v>0.001</v>
       </c>
       <c r="C12">
-        <v>2674.61</v>
+        <v>2789.06</v>
       </c>
       <c r="D12">
-        <v>81.05</v>
+        <v>84.52</v>
       </c>
       <c r="E12">
-        <v>1766.54</v>
+        <v>1857.1</v>
       </c>
       <c r="F12">
-        <v>53.53</v>
+        <v>56.28</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -626,16 +626,16 @@
         <v>0.001</v>
       </c>
       <c r="C13">
-        <v>1300.88</v>
+        <v>1522.54</v>
       </c>
       <c r="D13">
-        <v>39.42</v>
+        <v>46.14</v>
       </c>
       <c r="E13">
-        <v>-867.83</v>
+        <v>-902.6900000000001</v>
       </c>
       <c r="F13">
-        <v>-26.3</v>
+        <v>-27.35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -646,16 +646,16 @@
         <v>0.0001</v>
       </c>
       <c r="C14">
-        <v>808.88</v>
+        <v>744.79</v>
       </c>
       <c r="D14">
-        <v>24.51</v>
+        <v>22.57</v>
       </c>
       <c r="E14">
-        <v>887.59</v>
+        <v>798.35</v>
       </c>
       <c r="F14">
-        <v>26.9</v>
+        <v>24.19</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -666,16 +666,16 @@
         <v>0.0001</v>
       </c>
       <c r="C15">
-        <v>930.39</v>
+        <v>794.78</v>
       </c>
       <c r="D15">
-        <v>28.19</v>
+        <v>24.08</v>
       </c>
       <c r="E15">
-        <v>740.04</v>
+        <v>869.01</v>
       </c>
       <c r="F15">
-        <v>22.43</v>
+        <v>26.33</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -686,16 +686,16 @@
         <v>0.0001</v>
       </c>
       <c r="C16">
-        <v>121.51</v>
+        <v>49.99</v>
       </c>
       <c r="D16">
-        <v>3.68</v>
+        <v>1.51</v>
       </c>
       <c r="E16">
-        <v>-147.55</v>
+        <v>70.66</v>
       </c>
       <c r="F16">
-        <v>-4.47</v>
+        <v>2.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>